<commit_message>
Add is_contact; Fix #604
</commit_message>
<xml_diff>
--- a/docs/contributors/contributors.xlsx
+++ b/docs/contributors/contributors.xlsx
@@ -111,12 +111,25 @@
         </r>
       </text>
     </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Is this individual a contact for DOI purposes?</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>version</t>
   </si>
@@ -140,6 +153,9 @@
   </si>
   <si>
     <t>orcid_id</t>
+  </si>
+  <si>
+    <t>is_contact</t>
   </si>
 </sst>
 </file>
@@ -488,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -497,7 +513,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,11 +535,17 @@
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="H2:H1048576">
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>